<commit_message>
Adjusted plots and updated datastructures
</commit_message>
<xml_diff>
--- a/Files/raw/res-engelsk.xlsx
+++ b/Files/raw/res-engelsk.xlsx
@@ -119,57 +119,57 @@
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>windMun.Agder</t>
+          <t>windMun.42</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>windMun.Innlandet</t>
+          <t>windMun.34</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>windMun.Romsdal</t>
+          <t>windMun.15</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>windMun.Nordland</t>
+          <t>windMun.18</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>windMun.Oslo</t>
+          <t>windMun.03</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>windMun.Rogaland</t>
+          <t>windMun.11</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>windMun.Telemark</t>
+          <t>windMun.38</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>windMun.Finmark</t>
+          <t>windMun.54</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>windMun.Trondelag</t>
+          <t>windMun.50</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>windMun.Vestland</t>
+          <t>windMun.46</t>
         </is>
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>windMun.Viken</t>
+          <t>windMun.30</t>
         </is>
       </c>
       <c r="U1" t="inlineStr">
@@ -254,57 +254,57 @@
       </c>
       <c r="AK1" t="inlineStr">
         <is>
-          <t>sunPower.Agder</t>
+          <t>sunPower.42</t>
         </is>
       </c>
       <c r="AL1" t="inlineStr">
         <is>
-          <t>sunPower.Innlandet</t>
+          <t>sunPower.34</t>
         </is>
       </c>
       <c r="AM1" t="inlineStr">
         <is>
-          <t>sunPower.Romsdal</t>
+          <t>sunPower.15</t>
         </is>
       </c>
       <c r="AN1" t="inlineStr">
         <is>
-          <t>sunPower.Nordland</t>
+          <t>sunPower.18</t>
         </is>
       </c>
       <c r="AO1" t="inlineStr">
         <is>
-          <t>sunPower.Oslo</t>
+          <t>sunPower.03</t>
         </is>
       </c>
       <c r="AP1" t="inlineStr">
         <is>
-          <t>sunPower.Rogaland</t>
+          <t>sunPower.11</t>
         </is>
       </c>
       <c r="AQ1" t="inlineStr">
         <is>
-          <t>sunPower.Telemark</t>
+          <t>sunPower.38</t>
         </is>
       </c>
       <c r="AR1" t="inlineStr">
         <is>
-          <t>sunPower.Finmark</t>
+          <t>sunPower.54</t>
         </is>
       </c>
       <c r="AS1" t="inlineStr">
         <is>
-          <t>sunPower.Trondelag</t>
+          <t>sunPower.50</t>
         </is>
       </c>
       <c r="AT1" t="inlineStr">
         <is>
-          <t>sunPower.Vestland</t>
+          <t>sunPower.46</t>
         </is>
       </c>
       <c r="AU1" t="inlineStr">
         <is>
-          <t>sunPower.Viken</t>
+          <t>sunPower.30</t>
         </is>
       </c>
       <c r="AV1" t="inlineStr">

</xml_diff>